<commit_message>
push start year to 2019
</commit_message>
<xml_diff>
--- a/InputData/plcy-schd/IT/Initial Time.xlsx
+++ b/InputData/plcy-schd/IT/Initial Time.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivia\Documents\EPS_Models by Region\United States\us-eps\InputData\plcy-schd\IT\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivia\Documents\EPS_Models by Region\Canada\canada-eps\InputData\plcy-schd\IT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0DA93EC-B5DF-4DB0-97B6-F21DB44D41D9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC3F35F8-829B-4306-AE88-D68020855DE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12420" yWindow="840" windowWidth="15615" windowHeight="15645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8640" yWindow="1110" windowWidth="14730" windowHeight="12690" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -476,14 +476,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -491,52 +491,52 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
@@ -544,12 +544,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>16</v>
       </c>
@@ -557,12 +557,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>20</v>
       </c>
@@ -584,19 +584,19 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B1" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>4</v>
       </c>
       <c r="B2">
-        <v>2020</v>
+        <v>2019</v>
       </c>
     </row>
   </sheetData>

</xml_diff>